<commit_message>
updated the git checklist1
</commit_message>
<xml_diff>
--- a/Git-CheckList.xlsx
+++ b/Git-CheckList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="66">
   <si>
     <t>Git Check List</t>
   </si>
@@ -203,6 +203,15 @@
   </si>
   <si>
     <t>git config --global user.email &lt;"your_email@example.com"&gt;</t>
+  </si>
+  <si>
+    <t>clone the git remote repository to local reposiroty</t>
+  </si>
+  <si>
+    <t>git clone https://github.com/KrishnaGopalGupta/Git-Practice.git</t>
+  </si>
+  <si>
+    <t>git clone &lt;git remote url&gt;</t>
   </si>
 </sst>
 </file>
@@ -342,6 +351,10 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -351,10 +364,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,31 +671,31 @@
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="102.7109375" customWidth="1"/>
-    <col min="3" max="3" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -889,24 +898,24 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="3" t="s">
         <v>54</v>
       </c>
     </row>
@@ -944,9 +953,15 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="A26" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>

</xml_diff>